<commit_message>
multi wind scenarios generate
</commit_message>
<xml_diff>
--- a/wind_install.xlsx
+++ b/wind_install.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="市场预测" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -51,8 +52,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -371,11 +374,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="249147248"/>
-        <c:axId val="249148816"/>
+        <c:axId val="376875424"/>
+        <c:axId val="376875816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="249147248"/>
+        <c:axId val="376875424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,7 +421,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249148816"/>
+        <c:crossAx val="376875816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -426,7 +429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="249148816"/>
+        <c:axId val="376875816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120000"/>
@@ -478,7 +481,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249147248"/>
+        <c:crossAx val="376875424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -598,6 +601,744 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>2015-2019</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US"/>
+              <a:t>市场预测</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>年新增装机[GW]</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>市场预测!$A$1:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>市场预测!$B$1:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>51.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>累计装机[GW]</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>市场预测!$A$1:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>市场预测!$D$1:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>369.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>423.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>478.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>537.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>599.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>666.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="562709152"/>
+        <c:axId val="615536192"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>累计装机增长率</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>市场预测!$C$1:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0%">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.122</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.122</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11600000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>年新增装机增长率</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>市场预测!$E$1:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.442</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4000000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="497528128"/>
+        <c:axId val="497527736"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="562709152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="615536192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="255"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="615536192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="562709152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="497527736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="497528128"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="497528128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="497527736"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
   <a:schemeClr val="accent1"/>
@@ -635,7 +1376,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1171,6 +2455,81 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>471486</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="图表 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.00168</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.29735</cdr:x>
+      <cdr:y>0.06051</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="文本框 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="7824"/>
+          <a:ext cx="2085975" cy="273424"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>数据来源：全球风能理事会</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1462,8 +2821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1976" workbookViewId="0">
-      <selection activeCell="T2011" sqref="T2011"/>
+    <sheetView topLeftCell="A1976" workbookViewId="0">
+      <selection activeCell="A1986" sqref="A1986:S2017"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1683,4 +3042,123 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1">
+        <v>2014</v>
+      </c>
+      <c r="B1">
+        <v>51.5</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="D1">
+        <v>369.6</v>
+      </c>
+      <c r="E1" s="2">
+        <v>0.442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>2015</v>
+      </c>
+      <c r="B2">
+        <v>53.5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="D2">
+        <v>423.1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2016</v>
+      </c>
+      <c r="B3">
+        <v>55.5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="D3">
+        <v>478.6</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2017</v>
+      </c>
+      <c r="B4">
+        <v>58.5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.122</v>
+      </c>
+      <c r="D4">
+        <v>537.1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2018</v>
+      </c>
+      <c r="B5">
+        <v>62.5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.122</v>
+      </c>
+      <c r="D5">
+        <v>599.6</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>2019</v>
+      </c>
+      <c r="B6">
+        <v>66.5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="D6">
+        <v>666.1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>